<commit_message>
feat(compare): proof of concept
</commit_message>
<xml_diff>
--- a/src/__tests__/sample/Book1_versionA.xlsx
+++ b/src/__tests__/sample/Book1_versionA.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ldeparis\Documents\dev\excel\src\__tests__\sample\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718C9A73-749E-434F-BB8D-BFB3F3F0F3A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{693B2DA9-DA50-401C-93F9-F4B72C3E4CCD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{C8FCB4CB-3107-44A4-81F2-B43B9665CF09}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{C8FCB4CB-3107-44A4-81F2-B43B9665CF09}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2bis" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>Title</t>
   </si>
@@ -427,7 +428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A50233C0-6D03-4BC1-A9FC-BF7F219D0E95}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -539,4 +540,63 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E133A697-266F-4EEC-9581-7B9967F7BF82}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>44871</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>